<commit_message>
Actualizacion mejora Carga Masiva
</commit_message>
<xml_diff>
--- a/PLANTILLA_CREACION_USUARIOS.xlsx
+++ b/PLANTILLA_CREACION_USUARIOS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008E840D-D6C0-41D9-A7FD-3B330073E6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022C8C4F-E7F7-470C-8AF6-11A50B8A8A0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BE2EC2C-8EE0-41FB-ACB5-FC86299A78FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BE2EC2C-8EE0-41FB-ACB5-FC86299A78FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,10 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>NOMBRES</t>
   </si>
@@ -83,6 +78,45 @@
   </si>
   <si>
     <t>GUERRA</t>
+  </si>
+  <si>
+    <t>DOCENTE</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Ingeniería de Software</t>
+  </si>
+  <si>
+    <t>DASD</t>
+  </si>
+  <si>
+    <t>ASDASD</t>
+  </si>
+  <si>
+    <t>LA RASDASDOSA</t>
+  </si>
+  <si>
+    <t>RUBENSD</t>
+  </si>
+  <si>
+    <t>RUBENSAD</t>
+  </si>
+  <si>
+    <t>JIMENEZCCC</t>
+  </si>
+  <si>
+    <t>LA ROSACC</t>
+  </si>
+  <si>
+    <t>rjimenez@usmp.pe</t>
+  </si>
+  <si>
+    <t>rjimenez1@usmp.pe</t>
+  </si>
+  <si>
+    <t>rjimenez2@usmp.pe</t>
   </si>
 </sst>
 </file>
@@ -483,25 +517,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D2AB94-6003-4879-9E27-6DA8434878C7}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -530,7 +564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -547,33 +581,119 @@
         <v>11</v>
       </c>
       <c r="F2" s="1">
-        <v>100</v>
+        <v>1000000000</v>
       </c>
       <c r="G2" s="1">
-        <v>2426452</v>
+        <v>970599170</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>970599170</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>970599170</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <v>970599170</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{F4335B6B-2DF0-42BC-9449-5F3D023CBFB8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{F4335B6B-2DF0-42BC-9449-5F3D023CBFB8}">
       <formula1>"ALUMNO,DOCENTE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{2DD21E0C-7AB7-400E-8AF2-C4E82481ED5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5" xr:uid="{2DD21E0C-7AB7-400E-8AF2-C4E82481ED5B}">
       <formula1>"Ingeniería de Computación y Sistemas,Ingeniería de Software"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{99A4229B-5CD4-470E-A2A7-32E823091F91}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{99A4229B-5CD4-470E-A2A7-32E823091F91}">
       <formula1>"M,F"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E58E7748-4871-484C-AAF2-6D7D25212CD9}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{C0DFCB33-1099-4C0F-9D4B-BEAFA1DC0526}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{9FEB5515-C9CA-46EF-8C6C-D7606C2231D4}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{6F115928-B2AD-4E95-8FB2-ACB8D984641A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>